<commit_message>
Pruebas básicas con D3
Curso D3 + pruebas con visualización UNICAN
</commit_message>
<xml_diff>
--- a/VizUNICAN/Fuente_11 GR Egresados 1314 1415 v2.xlsx
+++ b/VizUNICAN/Fuente_11 GR Egresados 1314 1415 v2.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="533" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="533" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DatosBrutos" sheetId="2" r:id="rId1"/>
-    <sheet name="2015" sheetId="1" r:id="rId2"/>
-    <sheet name="2015-grafico" sheetId="4" r:id="rId3"/>
-    <sheet name="2015-grafico2" sheetId="5" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId2"/>
+    <sheet name="2015" sheetId="1" r:id="rId3"/>
+    <sheet name="2015-grafico" sheetId="4" r:id="rId4"/>
+    <sheet name="2015-grafico2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="55">
   <si>
     <t>EVOLUCIÓN ESTUDIANTES EGRESADOS EN ESTUDIOS DE GRADO</t>
   </si>
@@ -159,9 +160,6 @@
     <t>Curso 2015/16</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Mujeres</t>
   </si>
   <si>
@@ -177,19 +175,19 @@
     <t>EVOLUCIÓN ESTUDIANTES EGRESADOS EN ESTUDIOS DE GRADO 2014/15</t>
   </si>
   <si>
-    <t>Suma</t>
-  </si>
-  <si>
-    <t>Promedio</t>
-  </si>
-  <si>
-    <t>Cuenta</t>
-  </si>
-  <si>
     <t>Hombres</t>
   </si>
   <si>
     <t>Mujeres-</t>
+  </si>
+  <si>
+    <t>Ranking</t>
+  </si>
+  <si>
+    <t>Carrera</t>
+  </si>
+  <si>
+    <t>Categoría</t>
   </si>
 </sst>
 </file>
@@ -199,7 +197,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -211,6 +209,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -236,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,6 +248,11 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,26 +343,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l">
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI Black" panose="020B0A02040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI Black" panose="020B0A02040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI Black" panose="020B0A02040204020203" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -430,10 +419,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:layout/>
                 <c15:showLeaderLines val="0"/>
@@ -1199,12 +1184,7 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1387,11 +1367,11 @@
         </c:dLbls>
         <c:gapWidth val="25"/>
         <c:overlap val="100"/>
-        <c:axId val="492899824"/>
-        <c:axId val="492895120"/>
+        <c:axId val="256248728"/>
+        <c:axId val="256243240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="492899824"/>
+        <c:axId val="256248728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1437,7 +1417,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492895120"/>
+        <c:crossAx val="256243240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1445,7 +1425,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492895120"/>
+        <c:axId val="256243240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1455,7 +1435,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="492899824"/>
+        <c:crossAx val="256248728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2134,11 +2114,11 @@
         </c:dLbls>
         <c:gapWidth val="25"/>
         <c:overlap val="100"/>
-        <c:axId val="492896688"/>
-        <c:axId val="492901000"/>
+        <c:axId val="256247160"/>
+        <c:axId val="256245200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="492896688"/>
+        <c:axId val="256247160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2161,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492901000"/>
+        <c:crossAx val="256245200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2189,7 +2169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492901000"/>
+        <c:axId val="256245200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2230,7 +2210,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492896688"/>
+        <c:crossAx val="256247160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2307,46 +2287,6 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2891,511 +2831,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -3411,7 +2846,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3422,7 +2857,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6079537"/>
+    <xdr:ext cx="9305925" cy="6076950"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
@@ -3449,7 +2884,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9313333" cy="6079537"/>
+    <xdr:ext cx="9301574" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
@@ -3797,7 +3232,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3812,12 +3247,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:7">
       <c r="C2" t="s">
@@ -4591,17 +4026,17 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="7"/>
       <c r="G42" s="1">
         <v>20</v>
       </c>
@@ -4623,10 +4058,502 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3">
+        <v>24</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>11</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1">
+        <v>20</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3">
+        <v>9</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="1">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1">
+        <v>27</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>40</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1">
+        <v>62</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1">
+        <v>53</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1">
+        <v>94</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1">
+        <v>54</v>
+      </c>
+      <c r="D24" s="1">
+        <v>62</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3">
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1">
+        <v>97</v>
+      </c>
+      <c r="D25" s="1">
+        <v>43</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45</v>
+      </c>
+      <c r="D26" s="1">
+        <v>121</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:D26">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D66C8B10-80E3-4759-B88C-26A21F3A2554}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D66C8B10-80E3-4759-B88C-26A21F3A2554}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C2:D26</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G27" sqref="A3:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4641,27 +4568,27 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -4790,7 +4717,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="1">
-        <f>E8*-1</f>
+        <f t="shared" ref="C8:C27" si="0">E8*-1</f>
         <v>-4</v>
       </c>
       <c r="D8" s="1">
@@ -4814,7 +4741,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="1">
-        <f>E9*-1</f>
+        <f t="shared" si="0"/>
         <v>-7</v>
       </c>
       <c r="D9" s="1">
@@ -4838,7 +4765,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="1">
-        <f>E10*-1</f>
+        <f t="shared" si="0"/>
         <v>-4</v>
       </c>
       <c r="D10" s="1">
@@ -4862,7 +4789,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <f>E11*-1</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
       <c r="D11" s="1">
@@ -4886,7 +4813,7 @@
         <v>39</v>
       </c>
       <c r="C12" s="1">
-        <f>E12*-1</f>
+        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="D12" s="1">
@@ -4910,7 +4837,7 @@
         <v>35</v>
       </c>
       <c r="C13" s="1">
-        <f>E13*-1</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
       <c r="D13" s="1">
@@ -4934,7 +4861,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <f>E14*-1</f>
+        <f t="shared" si="0"/>
         <v>-11</v>
       </c>
       <c r="D14" s="1">
@@ -4958,7 +4885,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="1">
-        <f>E15*-1</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
       <c r="D15" s="1">
@@ -4982,7 +4909,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="1">
-        <f>E16*-1</f>
+        <f t="shared" si="0"/>
         <v>-20</v>
       </c>
       <c r="D16" s="1">
@@ -5006,7 +4933,7 @@
         <v>21</v>
       </c>
       <c r="C17" s="1">
-        <f>E17*-1</f>
+        <f t="shared" si="0"/>
         <v>-16</v>
       </c>
       <c r="D17" s="1">
@@ -5030,7 +4957,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="1">
-        <f>E18*-1</f>
+        <f t="shared" si="0"/>
         <v>-9</v>
       </c>
       <c r="D18" s="1">
@@ -5054,7 +4981,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="1">
-        <f>E19*-1</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
       <c r="D19" s="1">
@@ -5078,7 +5005,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="1">
-        <f>E20*-1</f>
+        <f t="shared" si="0"/>
         <v>-27</v>
       </c>
       <c r="D20" s="1">
@@ -5102,7 +5029,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="1">
-        <f>E21*-1</f>
+        <f t="shared" si="0"/>
         <v>-40</v>
       </c>
       <c r="D21" s="1">
@@ -5126,7 +5053,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="1">
-        <f>E22*-1</f>
+        <f t="shared" si="0"/>
         <v>-62</v>
       </c>
       <c r="D22" s="1">
@@ -5150,7 +5077,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="1">
-        <f>E23*-1</f>
+        <f t="shared" si="0"/>
         <v>-53</v>
       </c>
       <c r="D23" s="1">
@@ -5174,7 +5101,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="1">
-        <f>E24*-1</f>
+        <f t="shared" si="0"/>
         <v>-94</v>
       </c>
       <c r="D24" s="1">
@@ -5198,7 +5125,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="1">
-        <f>E25*-1</f>
+        <f t="shared" si="0"/>
         <v>-62</v>
       </c>
       <c r="D25" s="1">
@@ -5222,7 +5149,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="1">
-        <f>E26*-1</f>
+        <f t="shared" si="0"/>
         <v>-43</v>
       </c>
       <c r="D26" s="1">
@@ -5246,7 +5173,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="1">
-        <f>E27*-1</f>
+        <f t="shared" si="0"/>
         <v>-121</v>
       </c>
       <c r="D27" s="1">

</xml_diff>